<commit_message>
Changed () in [] in test instructions. Added Scopes_05 to demonstrate scope global combined with sid.
</commit_message>
<xml_diff>
--- a/Scopes_04.testcases.xlsx
+++ b/Scopes_04.testcases.xlsx
@@ -64,9 +64,9 @@
     <t>Vorbedingung prüfen</t>
   </si>
   <si>
-    <t>ET Testfall Vorbedingung (scope=global)
-B02 Testfall Vorbedingung (scope=global)
-A01 Testfall Vorbedingung (scope=global)
+    <t>ET Testfall Vorbedingung [scope global]
+B02 Testfall Vorbedingung [scope global]
+A01 Testfall Vorbedingung [scope global]
 B02/01 Testfall Vorbedingung
 A01/01 Testfall Vorbedingung</t>
   </si>
@@ -95,9 +95,9 @@
     <t>Nachbedingung prüfen</t>
   </si>
   <si>
-    <t>ET Testfall Nachbedingung (scope=global)
-B02 Testfall Nachbedingung (scope=global)
-A01 Testfall Nachbedingung (scope=global)
+    <t>ET Testfall Nachbedingung [scope global]
+B02 Testfall Nachbedingung [scope global]
+A01 Testfall Nachbedingung [scope global]
 B02/01 Testfall Nachbedingung
 A01/01 Testfall Nachbedingung</t>
   </si>
@@ -113,13 +113,13 @@
 | R04 | B03=J</t>
   </si>
   <si>
-    <t>ET Testfall Vorbedingung (scope=global)
-B02 Testfall Vorbedingung (scope=global)
-B04 Testfall Vorbedingung (scope=global)
-A01 Testfall Vorbedingung (scope=global)
-A02 Testfall Vorbedingung (scope=global)
-B03 Testfall Vorbedingung (scope=global)
-A01 Testfall Vorbedingung (scope=global)
+    <t>ET Testfall Vorbedingung [scope global]
+B02 Testfall Vorbedingung [scope global]
+B04 Testfall Vorbedingung [scope global]
+A01 Testfall Vorbedingung [scope global]
+A02 Testfall Vorbedingung [scope global]
+B03 Testfall Vorbedingung [scope global]
+A01 Testfall Vorbedingung [scope global]
 B02/02 Testfall Vorbedingung
 B04/01 Testfall Vorbedingung
 A01/01 Testfall Vorbedingung
@@ -152,13 +152,13 @@
     <t>B03/01 Erwartetes Resultat</t>
   </si>
   <si>
-    <t>ET Testfall Nachbedingung (scope=global)
-B02 Testfall Nachbedingung (scope=global)
-B04 Testfall Nachbedingung (scope=global)
-A01 Testfall Nachbedingung (scope=global)
-A02 Testfall Nachbedingung (scope=global)
-B03 Testfall Nachbedingung (scope=global)
-A01 Testfall Nachbedingung (scope=global)
+    <t>ET Testfall Nachbedingung [scope global]
+B02 Testfall Nachbedingung [scope global]
+B04 Testfall Nachbedingung [scope global]
+A01 Testfall Nachbedingung [scope global]
+A02 Testfall Nachbedingung [scope global]
+B03 Testfall Nachbedingung [scope global]
+A01 Testfall Nachbedingung [scope global]
 B02/02 Testfall Nachbedingung
 B04/01 Testfall Nachbedingung
 A01/01 Testfall Nachbedingung
@@ -178,15 +178,15 @@
 | R05 | B03=N | B04=J</t>
   </si>
   <si>
-    <t>ET Testfall Vorbedingung (scope=global)
-B02 Testfall Vorbedingung (scope=global)
-B04 Testfall Vorbedingung (scope=global)
-A01 Testfall Vorbedingung (scope=global)
-A02 Testfall Vorbedingung (scope=global)
-B03 Testfall Vorbedingung (scope=global)
-B04 Testfall Vorbedingung (scope=global)
-A01 Testfall Vorbedingung (scope=global)
-A02 Testfall Vorbedingung (scope=global)
+    <t>ET Testfall Vorbedingung [scope global]
+B02 Testfall Vorbedingung [scope global]
+B04 Testfall Vorbedingung [scope global]
+A01 Testfall Vorbedingung [scope global]
+A02 Testfall Vorbedingung [scope global]
+B03 Testfall Vorbedingung [scope global]
+B04 Testfall Vorbedingung [scope global]
+A01 Testfall Vorbedingung [scope global]
+A02 Testfall Vorbedingung [scope global]
 B02/02 Testfall Vorbedingung
 B04/01 Testfall Vorbedingung
 A01/01 Testfall Vorbedingung
@@ -203,15 +203,15 @@
     <t>B03/02 Erwartetes Resultat</t>
   </si>
   <si>
-    <t>ET Testfall Nachbedingung (scope=global)
-B02 Testfall Nachbedingung (scope=global)
-B04 Testfall Nachbedingung (scope=global)
-A01 Testfall Nachbedingung (scope=global)
-A02 Testfall Nachbedingung (scope=global)
-B03 Testfall Nachbedingung (scope=global)
-B04 Testfall Nachbedingung (scope=global)
-A01 Testfall Nachbedingung (scope=global)
-A02 Testfall Nachbedingung (scope=global)
+    <t>ET Testfall Nachbedingung [scope global]
+B02 Testfall Nachbedingung [scope global]
+B04 Testfall Nachbedingung [scope global]
+A01 Testfall Nachbedingung [scope global]
+A02 Testfall Nachbedingung [scope global]
+B03 Testfall Nachbedingung [scope global]
+B04 Testfall Nachbedingung [scope global]
+A01 Testfall Nachbedingung [scope global]
+A02 Testfall Nachbedingung [scope global]
 B02/02 Testfall Nachbedingung
 B04/01 Testfall Nachbedingung
 A01/01 Testfall Nachbedingung
@@ -233,12 +233,12 @@
 | R04 | B03=J</t>
   </si>
   <si>
-    <t>ET Testfall Vorbedingung (scope=global)
-B02 Testfall Vorbedingung (scope=global)
-B04 Testfall Vorbedingung (scope=global)
-A02 Testfall Vorbedingung (scope=global)
-B03 Testfall Vorbedingung (scope=global)
-A01 Testfall Vorbedingung (scope=global)
+    <t>ET Testfall Vorbedingung [scope global]
+B02 Testfall Vorbedingung [scope global]
+B04 Testfall Vorbedingung [scope global]
+A02 Testfall Vorbedingung [scope global]
+B03 Testfall Vorbedingung [scope global]
+A01 Testfall Vorbedingung [scope global]
 B02/02 Testfall Vorbedingung
 B04/02 Testfall Vorbedingung
 A02/01 Testfall Vorbedingung
@@ -252,12 +252,12 @@
     <t>B04/02 Erwartetes Resultat</t>
   </si>
   <si>
-    <t>ET Testfall Nachbedingung (scope=global)
-B02 Testfall Nachbedingung (scope=global)
-B04 Testfall Nachbedingung (scope=global)
-A02 Testfall Nachbedingung (scope=global)
-B03 Testfall Nachbedingung (scope=global)
-A01 Testfall Nachbedingung (scope=global)
+    <t>ET Testfall Nachbedingung [scope global]
+B02 Testfall Nachbedingung [scope global]
+B04 Testfall Nachbedingung [scope global]
+A02 Testfall Nachbedingung [scope global]
+B03 Testfall Nachbedingung [scope global]
+A01 Testfall Nachbedingung [scope global]
 B02/02 Testfall Nachbedingung
 B04/02 Testfall Nachbedingung
 A02/01 Testfall Nachbedingung
@@ -276,13 +276,13 @@
 | R06 | B03=N | B04=N</t>
   </si>
   <si>
-    <t>ET Testfall Vorbedingung (scope=global)
-B02 Testfall Vorbedingung (scope=global)
-B04 Testfall Vorbedingung (scope=global)
-A02 Testfall Vorbedingung (scope=global)
-B03 Testfall Vorbedingung (scope=global)
-B04 Testfall Vorbedingung (scope=global)
-A02 Testfall Vorbedingung (scope=global)
+    <t>ET Testfall Vorbedingung [scope global]
+B02 Testfall Vorbedingung [scope global]
+B04 Testfall Vorbedingung [scope global]
+A02 Testfall Vorbedingung [scope global]
+B03 Testfall Vorbedingung [scope global]
+B04 Testfall Vorbedingung [scope global]
+A02 Testfall Vorbedingung [scope global]
 B02/02 Testfall Vorbedingung
 B04/02 Testfall Vorbedingung
 A02/01 Testfall Vorbedingung
@@ -291,13 +291,13 @@
 A02/01 Testfall Vorbedingung</t>
   </si>
   <si>
-    <t>ET Testfall Nachbedingung (scope=global)
-B02 Testfall Nachbedingung (scope=global)
-B04 Testfall Nachbedingung (scope=global)
-A02 Testfall Nachbedingung (scope=global)
-B03 Testfall Nachbedingung (scope=global)
-B04 Testfall Nachbedingung (scope=global)
-A02 Testfall Nachbedingung (scope=global)
+    <t>ET Testfall Nachbedingung [scope global]
+B02 Testfall Nachbedingung [scope global]
+B04 Testfall Nachbedingung [scope global]
+A02 Testfall Nachbedingung [scope global]
+B03 Testfall Nachbedingung [scope global]
+B04 Testfall Nachbedingung [scope global]
+A02 Testfall Nachbedingung [scope global]
 B02/02 Testfall Nachbedingung
 B04/02 Testfall Nachbedingung
 A02/01 Testfall Nachbedingung
@@ -318,7 +318,7 @@
     <t>Aktuelles Verzeichnis (user.dir): "C:\Program Files\JetBrains\IntelliJ IDEA Community Edition 2022.1.2\jbr\bin"</t>
   </si>
   <si>
-    <t>Benötigte Zeit: 00:00:00.131 (25.03.2023 20:07:57.437 - 25.03.2023 20:07:57.568)</t>
+    <t>Benötigte Zeit: 00:00:00.707 (26.03.2023 14:47:43.668 - 26.03.2023 14:47:44.375)</t>
   </si>
   <si>
     <t>Entscheidungstabelle: D:\LF\Projekte\rulebased.group\lfet-examples-scope-de\Scopes_04.lfet</t>

</xml_diff>